<commit_message>
Feat: Add Hybrid mode and Judge rating system
</commit_message>
<xml_diff>
--- a/user_credential_and_analysis.xlsx
+++ b/user_credential_and_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a31b4ea5adb0516c/Desktop/excel_interviewer_ai/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_2B59D2BFD3E05A271FDA33115955D0735787FBBC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAF5859B-3E7E-4FE4-908D-960631B11CAD}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_2B59D2BFD35055580F393011597750B14D39E49B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7259520E-7FD5-41BB-8223-5B3279F2F35C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,11 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>username</t>
   </si>
   <si>
+    <t>interview_type</t>
+  </si>
+  <si>
     <t>test_taken</t>
   </si>
   <si>
@@ -52,13 +55,28 @@
     <t>evaluation_4</t>
   </si>
   <si>
-    <t>ninja1</t>
-  </si>
-  <si>
-    <t>ninja2</t>
-  </si>
-  <si>
-    <t>ninja3</t>
+    <t>final_rating</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>Static</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>Dynamic</t>
+  </si>
+  <si>
+    <t>user3</t>
+  </si>
+  <si>
+    <t>Hybrid</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -421,15 +439,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,40 +458,60 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix requirements for Streamlit deployment
</commit_message>
<xml_diff>
--- a/user_credential_and_analysis.xlsx
+++ b/user_credential_and_analysis.xlsx
@@ -1,105 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a31b4ea5adb0516c/Desktop/excel_interviewer_ai/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_2B59D2BFD35055580F393011597750B14D39E49B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7259520E-7FD5-41BB-8223-5B3279F2F35C}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>interview_type</t>
-  </si>
-  <si>
-    <t>test_taken</t>
-  </si>
-  <si>
-    <t>answer_1</t>
-  </si>
-  <si>
-    <t>evaluation_1</t>
-  </si>
-  <si>
-    <t>answer_2</t>
-  </si>
-  <si>
-    <t>evaluation_2</t>
-  </si>
-  <si>
-    <t>answer_3</t>
-  </si>
-  <si>
-    <t>evaluation_3</t>
-  </si>
-  <si>
-    <t>answer_4</t>
-  </si>
-  <si>
-    <t>evaluation_4</t>
-  </si>
-  <si>
-    <t>final_rating</t>
-  </si>
-  <si>
-    <t>user1</t>
-  </si>
-  <si>
-    <t>Static</t>
-  </si>
-  <si>
-    <t>user2</t>
-  </si>
-  <si>
-    <t>Dynamic</t>
-  </si>
-  <si>
-    <t>user3</t>
-  </si>
-  <si>
-    <t>Hybrid</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -114,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -438,81 +420,283 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>username</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>interview_type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>num_questions</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>test_taken</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>final_rating</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>answer_1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>evaluation_1</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>answer_2</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>evaluation_2</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>answer_3</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>evaluation_3</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>answer_4</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>evaluation_4</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>evaluation_5</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>answer_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>user1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Static</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="b">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>3/10</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Question: Let's start with a common one. Can you explain what the `VLOOKUP` function does in Excel and mention one of its main limitations?
+Evaluation: The candidate provided a correct and complete explanation of the VLOOKUP function, including its purpose, functionality, and a key limitation. They accurately described how VLOOKUP searches for a value in the leftmost column and retrieves data from a column to the right. The candidate also correctly identified the left-to-right lookup limitation. The additional point about column insertion/deletion is a good observation, although not strictly part of the core limitation being asked about. Overall, the answer demonstrates a solid understanding of VLOOKUP.
+Verdict: Correct</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Incorrect</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Question: Imagine you have a sales report with columns for 'Region', 'Product', and 'Sales Amount'. How would you calculate the total sales for the 'North' region for 'Laptops' only?
+Evaluation: The candidate explicitly stated their desire to skip the question, indicating an inability to answer. This demonstrates a lack of knowledge regarding the appropriate Excel functions for conditional summation. Therefore, the answer is incorrect.
+Verdict: Incorrect</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Incorrect</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Question: What are PivotTables in Excel, and what is their primary purpose?
+Evaluation: The candidate's answer demonstrates a superficial understanding of PivotTables. While they correctly identify that PivotTables involve "pivoting," they fail to articulate the core purpose of summarizing, analyzing, and exploring large datasets. The response lacks depth and doesn't convey the interactive and analytical capabilities that PivotTables offer.
+Verdict: Incorrect</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Incorrect</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Question: Why might an analyst prefer using `INDEX` and `MATCH` together instead of `VLOOKUP`?
+Evaluation: The candidate's answer is superficial and doesn't demonstrate a true understanding of the advantages of using `INDEX` and `MATCH` over `VLOOKUP`. While "easy to use," "time-efficient," and "user-friendly" might be subjective opinions, they don't address the core reasons for preferring `INDEX` and `MATCH`, such as the ability to look up values in any column or its stability when columns are inserted or deleted. The answer lacks the technical depth expected from someone proficient in Excel.
+Verdict: Incorrect</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>user2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Dynamic</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>user3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>user4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>user5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>user6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
hope it is final
</commit_message>
<xml_diff>
--- a/user_credential_and_analysis.xlsx
+++ b/user_credential_and_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a31b4ea5adb0516c/Desktop/excel_interviewer_ai/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_2B59D2BFD3E05561A75A2A11599798774B03E6C0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48FD73EE-B5B3-41E1-B19E-9C0B25F98762}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_2B59D2BFD390574DAB3B33115985B8B3758DE70B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0699B0AE-3099-4B9F-9807-C54969A6650D}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>username</t>
   </si>
@@ -71,35 +71,6 @@
   </si>
   <si>
     <t>Static</t>
-  </si>
-  <si>
-    <t>3/10</t>
-  </si>
-  <si>
-    <t>Correct</t>
-  </si>
-  <si>
-    <t>Question: Let's start with a common one. Can you explain what the `VLOOKUP` function does in Excel and mention one of its main limitations?
-Evaluation: The candidate provided a correct and complete explanation of the VLOOKUP function, including its purpose, functionality, and a key limitation. They accurately described how VLOOKUP searches for a value in the leftmost column and retrieves data from a column to the right. The candidate also correctly identified the left-to-right lookup limitation. The additional point about column insertion/deletion is a good observation, although not strictly part of the core limitation being asked about. Overall, the answer demonstrates a solid understanding of VLOOKUP.
-Verdict: Correct</t>
-  </si>
-  <si>
-    <t>Incorrect</t>
-  </si>
-  <si>
-    <t>Question: Imagine you have a sales report with columns for 'Region', 'Product', and 'Sales Amount'. How would you calculate the total sales for the 'North' region for 'Laptops' only?
-Evaluation: The candidate explicitly stated their desire to skip the question, indicating an inability to answer. This demonstrates a lack of knowledge regarding the appropriate Excel functions for conditional summation. Therefore, the answer is incorrect.
-Verdict: Incorrect</t>
-  </si>
-  <si>
-    <t>Question: What are PivotTables in Excel, and what is their primary purpose?
-Evaluation: The candidate's answer demonstrates a superficial understanding of PivotTables. While they correctly identify that PivotTables involve "pivoting," they fail to articulate the core purpose of summarizing, analyzing, and exploring large datasets. The response lacks depth and doesn't convey the interactive and analytical capabilities that PivotTables offer.
-Verdict: Incorrect</t>
-  </si>
-  <si>
-    <t>Question: Why might an analyst prefer using `INDEX` and `MATCH` together instead of `VLOOKUP`?
-Evaluation: The candidate's answer is superficial and doesn't demonstrate a true understanding of the advantages of using `INDEX` and `MATCH` over `VLOOKUP`. While "easy to use," "time-efficient," and "user-friendly" might be subjective opinions, they don't address the core reasons for preferring `INDEX` and `MATCH`, such as the ability to look up values in any column or its stability when columns are inserted or deleted. The answer lacks the technical depth expected from someone proficient in Excel.
-Verdict: Incorrect</t>
   </si>
   <si>
     <t>user2</t>
@@ -486,13 +457,10 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -548,43 +516,13 @@
       <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -592,10 +530,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -603,7 +541,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -611,18 +549,18 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>